<commit_message>
Figure tweaks, current responses
</commit_message>
<xml_diff>
--- a/ephyz/all-cell-ephyz-property-values-by-source.xlsx
+++ b/ephyz/all-cell-ephyz-property-values-by-source.xlsx
@@ -9,12 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24930" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Properties" sheetId="2" r:id="rId2"/>
+    <sheet name="Sources" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Properties!$A$89:$A$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sources!$A$1:$A$15</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="117">
   <si>
     <t>Stroh et al. (2012)</t>
   </si>
@@ -367,6 +372,15 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>Granule Cells</t>
+  </si>
+  <si>
+    <t>Mitral Cells</t>
+  </si>
+  <si>
+    <t>Tufted Cells</t>
   </si>
 </sst>
 </file>
@@ -415,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -433,8 +447,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C85" sqref="A24:C85"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -731,11 +754,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
@@ -924,11 +947,11 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="5"/>
@@ -1323,7 +1346,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B84" s="6" t="s">
@@ -1334,7 +1357,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A85" s="7"/>
+      <c r="A85" s="8"/>
       <c r="B85" s="6" t="s">
         <v>69</v>
       </c>
@@ -1343,11 +1366,11 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" s="5"/>
@@ -1562,14 +1585,689 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="1"/>
+      <c r="B4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="1"/>
+      <c r="B8" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B19" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A85" s="9"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A103" s="1"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A104" s="1"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A105" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A108"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1"/>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A15">
+    <sortState ref="A2:A15">
+      <sortCondition ref="A1:A108"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>